<commit_message>
login and sign up page is added
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -610,9 +610,35 @@
         <v>r444f56</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>DOC-1735824110933</v>
+      </c>
+      <c r="B9" t="str">
+        <v>sjfdhfs</v>
+      </c>
+      <c r="C9" t="str">
+        <v>2025-01-08</v>
+      </c>
+      <c r="D9" t="str">
+        <v>12:21</v>
+      </c>
+      <c r="E9" t="str">
+        <v>pdf</v>
+      </c>
+      <c r="F9" t="str">
+        <v>2025-01-15</v>
+      </c>
+      <c r="G9" t="str">
+        <v>14:32</v>
+      </c>
+      <c r="H9" t="str">
+        <v>aefa</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adition of the recive and forword action and the logs of the file is added
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -636,9 +636,61 @@
         <v>aefa</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>DOC-1735970018472</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Manvir</v>
+      </c>
+      <c r="C10" t="str">
+        <v>2025-01-08</v>
+      </c>
+      <c r="D10" t="str">
+        <v>14:02</v>
+      </c>
+      <c r="E10" t="str">
+        <v>manvir</v>
+      </c>
+      <c r="F10" t="str">
+        <v>0001-01-01</v>
+      </c>
+      <c r="G10" t="str">
+        <v>13:30</v>
+      </c>
+      <c r="H10" t="str">
+        <v>kdsfs</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>DOC-1735970506282</v>
+      </c>
+      <c r="B11" t="str">
+        <v>maa</v>
+      </c>
+      <c r="C11" t="str">
+        <v>2025-01-14</v>
+      </c>
+      <c r="D11" t="str">
+        <v>12:04</v>
+      </c>
+      <c r="E11" t="str">
+        <v>Manvir</v>
+      </c>
+      <c r="F11" t="str">
+        <v>2025-01-22</v>
+      </c>
+      <c r="G11" t="str">
+        <v>12:02</v>
+      </c>
+      <c r="H11" t="str">
+        <v>feds</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:H9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>